<commit_message>
Updated most important problem list with 10 new responses.
</commit_message>
<xml_diff>
--- a/data/mip_list.xlsx
+++ b/data/mip_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lauriercloud-my.sharepoint.com/personal/skiss_wlu_ca/Documents/projects_folder/public-health-canada/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crasy\OneDrive\Documents\public-health-canada-scott\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_A95FC044DCC9A284F605C6D9D568DF85230A05E7" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{52F63781-7FAD-1846-B3A5-B83992C4A117}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7D49DE-7101-4AF9-B924-B3342E8BFD85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22880" windowHeight="14920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10512" yWindow="1200" windowWidth="12984" windowHeight="10404" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="139">
   <si>
     <t>1 = COVID-19
 2 = Public health messaging/gov't handling of COVID
@@ -792,13 +792,13 @@
   <sheetViews>
     <sheetView topLeftCell="A95" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="77" customWidth="1"/>
     <col min="3" max="3" width="54.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -806,7 +806,7 @@
         <v>1944</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -823,7 +823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -840,7 +840,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -857,7 +857,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -874,7 +874,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -891,7 +891,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>0</v>
       </c>
@@ -908,7 +908,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -925,7 +925,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>0</v>
       </c>
@@ -942,7 +942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>0</v>
       </c>
@@ -959,7 +959,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>0</v>
       </c>
@@ -976,7 +976,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>0</v>
       </c>
@@ -993,7 +993,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>0</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>0</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>0</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>0</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>0</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>0</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>0</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>0</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>0</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>0</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>0</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>0</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>0</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>0</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>0</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>0</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>0</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>0</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>0</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>0</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>0</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>0</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>0</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>0</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>0</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>0</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>0</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>0</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>0</v>
       </c>
@@ -1503,7 +1503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>0</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>0</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>0</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>0</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>0</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>0</v>
       </c>
@@ -1605,7 +1605,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>0</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>0</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>0</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>0</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>0</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>0</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>0</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>0</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>0</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>0</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>0</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>0</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>0</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>0</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>0</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>0</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>0</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>0</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>0</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>0</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>0</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>0</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>0</v>
       </c>
@@ -1996,7 +1996,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>0</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>0</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>0</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>0</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
         <v>0</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
         <v>0</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
         <v>0</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
         <v>0</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
         <v>0</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
         <v>0</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
         <v>0</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>0</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>0</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
         <v>0</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
         <v>0</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
         <v>0</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>0</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>0</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>0</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>0</v>
       </c>
@@ -2336,7 +2336,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>0</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>0</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>0</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>0</v>
       </c>
@@ -2404,7 +2404,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>0</v>
       </c>
@@ -2421,7 +2421,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
         <v>0</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
         <v>0</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>0</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>0</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>0</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>0</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>0</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
         <v>0</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>0</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
         <v>0</v>
       </c>
@@ -2601,11 +2601,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B95" workbookViewId="0">
+      <selection activeCell="D114" sqref="D114"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="56.44140625" customWidth="1"/>
+    <col min="4" max="4" width="46" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>124</v>
       </c>
@@ -2625,7 +2631,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2645,7 +2651,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2665,7 +2671,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2685,7 +2691,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2705,7 +2711,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2725,7 +2731,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -2745,7 +2751,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2765,7 +2771,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2785,7 +2791,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2805,7 +2811,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2825,7 +2831,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -2845,7 +2851,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2865,7 +2871,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2885,7 +2891,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -2905,7 +2911,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -2925,7 +2931,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2945,7 +2951,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -2965,7 +2971,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2985,7 +2991,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -3005,7 +3011,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -3025,7 +3031,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -3045,7 +3051,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -3065,7 +3071,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -3085,7 +3091,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -3105,7 +3111,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -3125,7 +3131,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -3145,7 +3151,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -3165,7 +3171,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -3185,7 +3191,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -3205,7 +3211,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -3225,7 +3231,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -3245,7 +3251,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -3265,7 +3271,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -3285,7 +3291,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>48</v>
       </c>
@@ -3305,7 +3311,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>49</v>
       </c>
@@ -3325,7 +3331,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -3345,7 +3351,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -3365,7 +3371,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>52</v>
       </c>
@@ -3385,7 +3391,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -3405,7 +3411,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -3425,7 +3431,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -3445,7 +3451,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -3465,7 +3471,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -3485,7 +3491,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>59</v>
       </c>
@@ -3505,7 +3511,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -3525,7 +3531,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -3545,7 +3551,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>62</v>
       </c>
@@ -3565,7 +3571,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -3585,7 +3591,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -3605,7 +3611,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -3625,7 +3631,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -3645,7 +3651,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>67</v>
       </c>
@@ -3665,7 +3671,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>68</v>
       </c>
@@ -3685,7 +3691,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>70</v>
       </c>
@@ -3705,7 +3711,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>71</v>
       </c>
@@ -3725,7 +3731,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>73</v>
       </c>
@@ -3745,7 +3751,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>75</v>
       </c>
@@ -3765,7 +3771,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>76</v>
       </c>
@@ -3785,7 +3791,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>77</v>
       </c>
@@ -3805,7 +3811,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>78</v>
       </c>
@@ -3825,7 +3831,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>79</v>
       </c>
@@ -3845,7 +3851,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>80</v>
       </c>
@@ -3865,7 +3871,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>81</v>
       </c>
@@ -3885,7 +3891,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>82</v>
       </c>
@@ -3905,7 +3911,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>83</v>
       </c>
@@ -3925,7 +3931,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>84</v>
       </c>
@@ -3945,7 +3951,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>85</v>
       </c>
@@ -3965,7 +3971,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>86</v>
       </c>
@@ -3985,7 +3991,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>87</v>
       </c>
@@ -4005,7 +4011,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>88</v>
       </c>
@@ -4025,7 +4031,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>89</v>
       </c>
@@ -4045,7 +4051,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>90</v>
       </c>
@@ -4065,7 +4071,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>91</v>
       </c>
@@ -4085,7 +4091,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>92</v>
       </c>
@@ -4105,7 +4111,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>93</v>
       </c>
@@ -4125,7 +4131,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>94</v>
       </c>
@@ -4145,7 +4151,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>95</v>
       </c>
@@ -4165,7 +4171,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>96</v>
       </c>
@@ -4185,7 +4191,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>97</v>
       </c>
@@ -4205,7 +4211,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>98</v>
       </c>
@@ -4225,7 +4231,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>99</v>
       </c>
@@ -4245,7 +4251,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>100</v>
       </c>
@@ -4265,7 +4271,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>101</v>
       </c>
@@ -4285,7 +4291,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>102</v>
       </c>
@@ -4305,7 +4311,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>103</v>
       </c>
@@ -4325,7 +4331,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>104</v>
       </c>
@@ -4345,7 +4351,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>105</v>
       </c>
@@ -4365,7 +4371,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>106</v>
       </c>
@@ -4385,7 +4391,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>107</v>
       </c>
@@ -4405,7 +4411,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>108</v>
       </c>
@@ -4425,7 +4431,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>109</v>
       </c>
@@ -4445,7 +4451,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>110</v>
       </c>
@@ -4465,7 +4471,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>111</v>
       </c>
@@ -4485,7 +4491,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>112</v>
       </c>
@@ -4505,7 +4511,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>113</v>
       </c>
@@ -4525,7 +4531,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>114</v>
       </c>
@@ -4545,7 +4551,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>115</v>
       </c>
@@ -4565,7 +4571,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>116</v>
       </c>
@@ -4585,7 +4591,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>117</v>
       </c>
@@ -4605,7 +4611,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>118</v>
       </c>
@@ -4625,7 +4631,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>119</v>
       </c>
@@ -4645,7 +4651,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>120</v>
       </c>
@@ -4665,7 +4671,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>121</v>
       </c>
@@ -4685,7 +4691,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>122</v>
       </c>
@@ -4705,7 +4711,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>123</v>
       </c>
@@ -4725,7 +4731,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>130</v>
       </c>
@@ -4736,10 +4742,16 @@
         <v>130</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>131</v>
       </c>
+      <c r="C108">
+        <v>6</v>
+      </c>
+      <c r="D108" t="s">
+        <v>34</v>
+      </c>
       <c r="E108">
         <v>1</v>
       </c>
@@ -4747,10 +4759,16 @@
         <v>130</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>132</v>
       </c>
+      <c r="C109">
+        <v>2</v>
+      </c>
+      <c r="D109" t="s">
+        <v>25</v>
+      </c>
       <c r="E109">
         <v>1</v>
       </c>
@@ -4758,10 +4776,16 @@
         <v>130</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>133</v>
       </c>
+      <c r="C110">
+        <v>5</v>
+      </c>
+      <c r="D110" t="s">
+        <v>10</v>
+      </c>
       <c r="E110">
         <v>1</v>
       </c>
@@ -4769,10 +4793,16 @@
         <v>130</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>134</v>
       </c>
+      <c r="C111">
+        <v>7</v>
+      </c>
+      <c r="D111" t="s">
+        <v>4</v>
+      </c>
       <c r="E111">
         <v>1</v>
       </c>
@@ -4780,10 +4810,16 @@
         <v>130</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>135</v>
       </c>
+      <c r="C112">
+        <v>7</v>
+      </c>
+      <c r="D112" t="s">
+        <v>4</v>
+      </c>
       <c r="E112">
         <v>1</v>
       </c>
@@ -4791,10 +4827,16 @@
         <v>130</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>136</v>
       </c>
+      <c r="C113">
+        <v>7</v>
+      </c>
+      <c r="D113" t="s">
+        <v>4</v>
+      </c>
       <c r="E113">
         <v>1</v>
       </c>
@@ -4802,10 +4844,16 @@
         <v>130</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>137</v>
       </c>
+      <c r="C114">
+        <v>2</v>
+      </c>
+      <c r="D114" t="s">
+        <v>34</v>
+      </c>
       <c r="E114">
         <v>1</v>
       </c>
@@ -4813,9 +4861,15 @@
         <v>130</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>138</v>
+      </c>
+      <c r="C115">
+        <v>9</v>
+      </c>
+      <c r="D115" t="s">
+        <v>69</v>
       </c>
       <c r="E115">
         <v>1</v>

</xml_diff>

<commit_message>
Updated with index of answers.
</commit_message>
<xml_diff>
--- a/data/mip_list.xlsx
+++ b/data/mip_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crasy\OneDrive\Documents\public-health-canada-scott\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7D49DE-7101-4AF9-B924-B3342E8BFD85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A63F88-47D6-4B05-BDE5-9E45AA38F889}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10512" yWindow="1200" windowWidth="12984" windowHeight="10404" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="158">
   <si>
     <t>1 = COVID-19
 2 = Public health messaging/gov't handling of COVID
@@ -455,6 +455,63 @@
   </si>
   <si>
     <t>racism</t>
+  </si>
+  <si>
+    <t>1 = COVID-19</t>
+  </si>
+  <si>
+    <t>2 = Public health messaging/gov't handling of COVID</t>
+  </si>
+  <si>
+    <t>3 = Healthcare (access to care, short supply)</t>
+  </si>
+  <si>
+    <t>4 = Long term care</t>
+  </si>
+  <si>
+    <t>5 = Chronic disease (cancer, heart disease)</t>
+  </si>
+  <si>
+    <t>6 = Mental health</t>
+  </si>
+  <si>
+    <t>7 = Access to housing and food</t>
+  </si>
+  <si>
+    <t>8 = Drug abuse</t>
+  </si>
+  <si>
+    <t>9 = Inequality</t>
+  </si>
+  <si>
+    <t>10 = Economy</t>
+  </si>
+  <si>
+    <t>11 = Corrupt gov't</t>
+  </si>
+  <si>
+    <t>12 = Climate change/environmental</t>
+  </si>
+  <si>
+    <t>13 = Abortion</t>
+  </si>
+  <si>
+    <t>14 = Reliance on meat</t>
+  </si>
+  <si>
+    <t>15 = Domestic abuse</t>
+  </si>
+  <si>
+    <t>16 = Misinformation</t>
+  </si>
+  <si>
+    <t>17 = Internet addiction</t>
+  </si>
+  <si>
+    <t>18 = Don't know</t>
+  </si>
+  <si>
+    <t>index</t>
   </si>
 </sst>
 </file>
@@ -2599,19 +2656,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F115"/>
+  <dimension ref="A1:I115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B95" workbookViewId="0">
-      <selection activeCell="D114" sqref="D114"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="56.44140625" customWidth="1"/>
+    <col min="1" max="1" width="51.21875" customWidth="1"/>
     <col min="4" max="4" width="46" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>124</v>
       </c>
@@ -2630,8 +2688,11 @@
       <c r="F1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2650,8 +2711,11 @@
       <c r="F2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2670,8 +2734,11 @@
       <c r="F3" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2690,8 +2757,11 @@
       <c r="F4" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2710,8 +2780,11 @@
       <c r="F5" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2730,8 +2803,11 @@
       <c r="F6" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -2750,8 +2826,11 @@
       <c r="F7" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2770,8 +2849,11 @@
       <c r="F8" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2790,8 +2872,11 @@
       <c r="F9" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2810,8 +2895,11 @@
       <c r="F10" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2830,8 +2918,11 @@
       <c r="F11" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -2850,8 +2941,11 @@
       <c r="F12" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2870,8 +2964,11 @@
       <c r="F13" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2890,8 +2987,11 @@
       <c r="F14" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -2910,8 +3010,11 @@
       <c r="F15" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -2930,8 +3033,11 @@
       <c r="F16" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2950,8 +3056,11 @@
       <c r="F17" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -2970,8 +3079,11 @@
       <c r="F18" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2990,8 +3102,11 @@
       <c r="F19" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -3011,7 +3126,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -3031,7 +3146,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -3051,7 +3166,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -3071,7 +3186,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -3091,7 +3206,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -3111,7 +3226,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -3131,7 +3246,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -3151,7 +3266,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -3171,7 +3286,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -3191,7 +3306,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -3211,7 +3326,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -3231,7 +3346,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
Uploaded Scott's MIP changes, added variable labels to dichotomous variables
</commit_message>
<xml_diff>
--- a/data/mip_list.xlsx
+++ b/data/mip_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lauriercloud-my.sharepoint.com/personal/skiss_wlu_ca/Documents/projects_folder/public-health-canada/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skiss/OneDrive - Wilfrid Laurier University/projects_folder/public-health-canada/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_A95FC044DCC9A284F605C6D9D568DF85230A05E7" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{52F63781-7FAD-1846-B3A5-B83992C4A117}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C430562-D1B2-D445-B12D-F3112FC2860C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22880" windowHeight="14920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="158">
   <si>
     <t>1 = COVID-19
 2 = Public health messaging/gov't handling of COVID
@@ -455,6 +455,63 @@
   </si>
   <si>
     <t>racism</t>
+  </si>
+  <si>
+    <t>1 = COVID-19</t>
+  </si>
+  <si>
+    <t>2 = Public health messaging/gov't handling of COVID</t>
+  </si>
+  <si>
+    <t>3 = Healthcare (access to care, short supply)</t>
+  </si>
+  <si>
+    <t>4 = Long term care</t>
+  </si>
+  <si>
+    <t>5 = Chronic disease (cancer, heart disease)</t>
+  </si>
+  <si>
+    <t>6 = Mental health</t>
+  </si>
+  <si>
+    <t>7 = Access to housing and food</t>
+  </si>
+  <si>
+    <t>8 = Drug abuse</t>
+  </si>
+  <si>
+    <t>9 = Inequality</t>
+  </si>
+  <si>
+    <t>10 = Economy</t>
+  </si>
+  <si>
+    <t>11 = Corrupt gov't</t>
+  </si>
+  <si>
+    <t>12 = Climate change/environmental</t>
+  </si>
+  <si>
+    <t>13 = Abortion</t>
+  </si>
+  <si>
+    <t>14 = Reliance on meat</t>
+  </si>
+  <si>
+    <t>15 = Domestic abuse</t>
+  </si>
+  <si>
+    <t>16 = Misinformation</t>
+  </si>
+  <si>
+    <t>17 = Internet addiction</t>
+  </si>
+  <si>
+    <t>18 = Don't know</t>
+  </si>
+  <si>
+    <t>index</t>
   </si>
 </sst>
 </file>
@@ -790,9 +847,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:F106"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0"/>
+    <sheetView topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="77" customWidth="1"/>
     <col min="3" max="3" width="54.6640625" customWidth="1"/>
@@ -2599,13 +2658,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F115"/>
+  <dimension ref="A1:I114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="51.1640625" customWidth="1"/>
+    <col min="4" max="4" width="46" customWidth="1"/>
+    <col min="9" max="9" width="13.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>124</v>
       </c>
@@ -2624,8 +2690,11 @@
       <c r="F1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2644,8 +2713,11 @@
       <c r="F2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2664,8 +2736,11 @@
       <c r="F3" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -2684,8 +2759,11 @@
       <c r="F4" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2704,8 +2782,11 @@
       <c r="F5" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2724,8 +2805,11 @@
       <c r="F6" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -2744,8 +2828,11 @@
       <c r="F7" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2764,8 +2851,11 @@
       <c r="F8" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2784,8 +2874,11 @@
       <c r="F9" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2804,8 +2897,11 @@
       <c r="F10" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2824,8 +2920,11 @@
       <c r="F11" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -2844,8 +2943,11 @@
       <c r="F12" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2864,8 +2966,11 @@
       <c r="F13" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2884,8 +2989,11 @@
       <c r="F14" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -2904,8 +3012,11 @@
       <c r="F15" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I15" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -2924,8 +3035,11 @@
       <c r="F16" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -2944,8 +3058,11 @@
       <c r="F17" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -2964,8 +3081,11 @@
       <c r="F18" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -2984,8 +3104,11 @@
       <c r="F19" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -3005,7 +3128,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -3025,7 +3148,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -3045,7 +3168,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -3065,7 +3188,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -3085,7 +3208,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -3105,7 +3228,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -3125,7 +3248,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -3145,7 +3268,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -3165,7 +3288,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -3185,7 +3308,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -3205,7 +3328,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>44</v>
       </c>
@@ -3225,7 +3348,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -4150,10 +4273,10 @@
         <v>95</v>
       </c>
       <c r="B78">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C78">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D78" t="s">
         <v>22</v>
@@ -4253,7 +4376,7 @@
         <v>3</v>
       </c>
       <c r="C83">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D83" t="s">
         <v>22</v>
@@ -4273,7 +4396,7 @@
         <v>1</v>
       </c>
       <c r="C84">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D84" t="s">
         <v>22</v>
@@ -4333,7 +4456,7 @@
         <v>2</v>
       </c>
       <c r="C87">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D87" t="s">
         <v>22</v>
@@ -4493,7 +4616,7 @@
         <v>1</v>
       </c>
       <c r="C95">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D95" t="s">
         <v>22</v>
@@ -4727,10 +4850,16 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>130</v>
+        <v>131</v>
+      </c>
+      <c r="C107">
+        <v>6</v>
+      </c>
+      <c r="D107" t="s">
+        <v>34</v>
       </c>
       <c r="E107">
-        <v>2056</v>
+        <v>1</v>
       </c>
       <c r="F107" t="s">
         <v>130</v>
@@ -4738,7 +4867,13 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="C108">
+        <v>2</v>
+      </c>
+      <c r="D108" t="s">
+        <v>25</v>
       </c>
       <c r="E108">
         <v>1</v>
@@ -4749,7 +4884,13 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>132</v>
+        <v>133</v>
+      </c>
+      <c r="C109">
+        <v>5</v>
+      </c>
+      <c r="D109" t="s">
+        <v>10</v>
       </c>
       <c r="E109">
         <v>1</v>
@@ -4760,7 +4901,13 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>133</v>
+        <v>134</v>
+      </c>
+      <c r="C110">
+        <v>7</v>
+      </c>
+      <c r="D110" t="s">
+        <v>4</v>
       </c>
       <c r="E110">
         <v>1</v>
@@ -4771,7 +4918,13 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>134</v>
+        <v>135</v>
+      </c>
+      <c r="C111">
+        <v>7</v>
+      </c>
+      <c r="D111" t="s">
+        <v>4</v>
       </c>
       <c r="E111">
         <v>1</v>
@@ -4782,7 +4935,13 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>135</v>
+        <v>136</v>
+      </c>
+      <c r="C112">
+        <v>7</v>
+      </c>
+      <c r="D112" t="s">
+        <v>4</v>
       </c>
       <c r="E112">
         <v>1</v>
@@ -4793,7 +4952,13 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>136</v>
+        <v>137</v>
+      </c>
+      <c r="C113">
+        <v>2</v>
+      </c>
+      <c r="D113" t="s">
+        <v>34</v>
       </c>
       <c r="E113">
         <v>1</v>
@@ -4804,23 +4969,18 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>137</v>
+        <v>138</v>
+      </c>
+      <c r="C114">
+        <v>9</v>
+      </c>
+      <c r="D114" t="s">
+        <v>69</v>
       </c>
       <c r="E114">
         <v>1</v>
       </c>
       <c r="F114" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
-        <v>138</v>
-      </c>
-      <c r="E115">
-        <v>1</v>
-      </c>
-      <c r="F115" t="s">
         <v>130</v>
       </c>
     </row>

</xml_diff>